<commit_message>
Final version with excel
</commit_message>
<xml_diff>
--- a/baza.xlsx
+++ b/baza.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepi\MyJavaProjects\LoginThymeleafSB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D003D1D-2AD9-478D-846D-D13755202EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86C9727-87C5-4866-9155-A03EFD007DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,33 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Wiktor</t>
   </si>
   <si>
-    <t>Stępień</t>
-  </si>
-  <si>
     <t>Maciej</t>
   </si>
   <si>
-    <t>Beraś</t>
-  </si>
-  <si>
     <t xml:space="preserve">Luiza </t>
   </si>
   <si>
-    <t>Grędziel</t>
-  </si>
-  <si>
-    <t>wiktorstepien@gmail.com</t>
-  </si>
-  <si>
-    <t>maciejberas@gmail.com</t>
-  </si>
-  <si>
-    <t>luizagradziel@gmail.com</t>
+    <t>Kowalski</t>
+  </si>
+  <si>
+    <t>Kowalska</t>
+  </si>
+  <si>
+    <t>wiktorkowalski1@gmail.com</t>
+  </si>
+  <si>
+    <t>maciejkowalski1@gmail.com</t>
+  </si>
+  <si>
+    <t>luizakowalska1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -383,7 +380,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,10 +393,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1">
         <v>1000</v>
@@ -410,13 +407,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>2000</v>
@@ -427,13 +424,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>3000</v>

</xml_diff>